<commit_message>
Additional stats - correct lmer comparisons + CIs
</commit_message>
<xml_diff>
--- a/Comprehension - GesturetoSentence/graphs 2-6-14.xlsx
+++ b/Comprehension - GesturetoSentence/graphs 2-6-14.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
   <si>
     <t>All items</t>
   </si>
@@ -88,6 +88,45 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>&gt; quantile(PersonSOV.boot.mean$thetastar, c(0.025, 0.975))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.5%    97.5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.104762 8.914286 </t>
+  </si>
+  <si>
+    <t>&gt; PersonSVO.boot.mean = bootstrap(Scores[Scores$sentType=="AO" &amp; Scores$sentOrder=="SVO",]$CorrectScore, 1000, mean)</t>
+  </si>
+  <si>
+    <t>&gt; quantile(PersonSVO.boot.mean$thetastar, c(0.025, 0.975))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.866667 9.752381 </t>
+  </si>
+  <si>
+    <t>&gt; ObjectSOV.boot.mean = bootstrap(Scores[Scores$sentType=="IO" &amp; Scores$sentOrder=="SOV",]$CorrectScore, 1000, mean)</t>
+  </si>
+  <si>
+    <t>&gt; quantile(ObjectSOV.boot.mean$thetastar, c(0.025, 0.975))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.628571 9.505238 </t>
+  </si>
+  <si>
+    <t>&gt; ObjectSVO.boot.mean = bootstrap(Scores[Scores$sentType=="IO" &amp; Scores$sentOrder=="SVO",]$CorrectScore, 1000, mean)</t>
+  </si>
+  <si>
+    <t>&gt; quantile(ObjectSVO.boot.mean$thetastar, c(0.025, 0.975))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.161905 9.952381 </t>
+  </si>
+  <si>
+    <t>New error bars!  Bootstrapped Cis</t>
   </si>
 </sst>
 </file>
@@ -398,11 +437,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2121918280"/>
-        <c:axId val="2108743864"/>
+        <c:axId val="2110326008"/>
+        <c:axId val="2114804824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121918280"/>
+        <c:axId val="2110326008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -411,7 +450,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108743864"/>
+        <c:crossAx val="2114804824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -419,7 +458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108743864"/>
+        <c:axId val="2114804824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,7 +492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121918280"/>
+        <c:crossAx val="2110326008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -664,11 +703,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2107316936"/>
-        <c:axId val="-2121724984"/>
+        <c:axId val="2109693032"/>
+        <c:axId val="2109524184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107316936"/>
+        <c:axId val="2109693032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,7 +716,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121724984"/>
+        <c:crossAx val="2109524184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -685,7 +724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121724984"/>
+        <c:axId val="2109524184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107316936"/>
+        <c:crossAx val="2109693032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -907,11 +946,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110326984"/>
-        <c:axId val="2110232408"/>
+        <c:axId val="2107607240"/>
+        <c:axId val="2109382184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110326984"/>
+        <c:axId val="2107607240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110232408"/>
+        <c:crossAx val="2109382184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -928,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110232408"/>
+        <c:axId val="2109382184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110326984"/>
+        <c:crossAx val="2107607240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1150,11 +1189,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2121920696"/>
-        <c:axId val="-2121922856"/>
+        <c:axId val="-2121051656"/>
+        <c:axId val="-2121169352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121920696"/>
+        <c:axId val="-2121051656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1163,7 +1202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121922856"/>
+        <c:crossAx val="-2121169352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1171,7 +1210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121922856"/>
+        <c:axId val="-2121169352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -1184,7 +1223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121920696"/>
+        <c:crossAx val="-2121051656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1337,11 +1376,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2114773208"/>
-        <c:axId val="-2121911160"/>
+        <c:axId val="2110240408"/>
+        <c:axId val="2114217000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2114773208"/>
+        <c:axId val="2110240408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121911160"/>
+        <c:crossAx val="2114217000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1358,7 +1397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121911160"/>
+        <c:axId val="2114217000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -1371,14 +1410,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114773208"/>
+        <c:crossAx val="2110240408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1445,10 +1483,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.21</c:v>
+                    <c:v>0.405</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.21</c:v>
+                    <c:v>0.44</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1460,10 +1498,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.21</c:v>
+                    <c:v>0.405</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.21</c:v>
+                    <c:v>0.44</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1530,10 +1568,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.22</c:v>
+                    <c:v>0.435</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.21</c:v>
+                    <c:v>0.395</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1545,10 +1583,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.22</c:v>
+                    <c:v>0.435</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.21</c:v>
+                    <c:v>0.395</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1593,11 +1631,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2114569096"/>
-        <c:axId val="2109278392"/>
+        <c:axId val="-2120854360"/>
+        <c:axId val="-2120863736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2114569096"/>
+        <c:axId val="-2120854360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109278392"/>
+        <c:crossAx val="-2120863736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1614,7 +1652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109278392"/>
+        <c:axId val="-2120863736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12.0"/>
@@ -1627,7 +1665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114569096"/>
+        <c:crossAx val="-2120854360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2564,15 +2602,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:K7"/>
+  <dimension ref="B1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="5:11">
+    <row r="1" spans="2:11">
       <c r="E1" t="s">
         <v>12</v>
       </c>
@@ -2583,7 +2621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="5:11">
+    <row r="2" spans="2:11">
       <c r="E2" t="s">
         <v>13</v>
       </c>
@@ -2600,7 +2638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="5:11">
+    <row r="3" spans="2:11">
       <c r="E3" t="s">
         <v>14</v>
       </c>
@@ -2614,7 +2652,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="5:11">
+    <row r="5" spans="2:11">
       <c r="E5" t="s">
         <v>15</v>
       </c>
@@ -2628,7 +2666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="5:11">
+    <row r="6" spans="2:11">
       <c r="E6" t="s">
         <v>16</v>
       </c>
@@ -2636,13 +2674,15 @@
         <v>18</v>
       </c>
       <c r="H6">
-        <v>0.21</v>
+        <f>(8.91-8.1)/2</f>
+        <v>0.40500000000000025</v>
       </c>
       <c r="I6">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="7" spans="5:11">
+        <f>(9.75-8.87)/2</f>
+        <v>0.44000000000000039</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="E7" t="s">
         <v>17</v>
       </c>
@@ -2650,10 +2690,92 @@
         <v>19</v>
       </c>
       <c r="H7">
-        <v>0.22</v>
+        <f>(9.5-8.63)/2</f>
+        <v>0.43499999999999961</v>
       </c>
       <c r="I7">
-        <v>0.21</v>
+        <f>(9.95-9.16)/2</f>
+        <v>0.39499999999999957</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>